<commit_message>
Another DB div and results in excel
</commit_message>
<xml_diff>
--- a/Wyniki.xlsx
+++ b/Wyniki.xlsx
@@ -24,30 +24,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Ludzie</t>
   </si>
   <si>
-    <t>Krysian</t>
+    <t>SVM</t>
   </si>
   <si>
-    <t>Sebastian</t>
+    <t>NN-class</t>
   </si>
   <si>
-    <t>Rafał G.</t>
+    <t>Close-body</t>
   </si>
   <si>
-    <t>Rafał P.</t>
+    <t>Far-body</t>
   </si>
   <si>
-    <t>Bartek</t>
+    <t>Head</t>
   </si>
   <si>
-    <t>Marcin</t>
-  </si>
-  <si>
-    <t>Komputer(SVM)</t>
+    <t>Medium-body</t>
   </si>
 </sst>
 </file>
@@ -117,11 +114,12 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -138,28 +136,34 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:numRef>
-              <c:f>Arkusz1!$C$2</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+            <c:strRef>
+              <c:f>Arkusz1!$A$2:$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.76068380000000002</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v>Close-body</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Far-body</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Head</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Medium-body</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -168,15 +172,11 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.92</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.86</c:v>
+                  <c:v>0.94</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -187,23 +187,41 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Komputer(SVM)</c:v>
+                  <c:v>SVM</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Arkusz1!$A$2:$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Close-body</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Far-body</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Head</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Medium-body</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Arkusz1!$C$2:$C$5</c:f>
@@ -211,21 +229,74 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.76068380000000002</c:v>
+                  <c:v>0.8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.76068380000000002</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.76068380000000002</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.76068380000000002</c:v>
+                  <c:v>0.63</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Arkusz1!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>NN-class</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Arkusz1!$A$2:$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Close-body</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Far-body</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Head</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Medium-body</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Arkusz1!$D$2:$D$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.72</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.48</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -235,22 +306,69 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="-84352176"/>
-        <c:axId val="-84355984"/>
-      </c:lineChart>
+        <c:gapWidth val="150"/>
+        <c:axId val="-320594224"/>
+        <c:axId val="-487423904"/>
+      </c:barChart>
       <c:catAx>
-        <c:axId val="-84352176"/>
+        <c:axId val="-320594224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="1"/>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-84355984"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-487423904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -258,7 +376,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-84355984"/>
+        <c:axId val="-487423904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -284,8 +402,14 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln>
-            <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -309,7 +433,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-84352176"/>
+        <c:crossAx val="-320594224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -322,7 +446,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="r"/>
+      <c:legendPos val="b"/>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -431,7 +555,7 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -458,8 +582,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -539,11 +663,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -554,11 +673,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -570,7 +684,7 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+      <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -590,9 +704,6 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -605,10 +716,10 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -648,22 +759,23 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -768,8 +880,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -901,19 +1013,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -927,6 +1040,17 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -950,20 +1074,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>119062</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>885824</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>100011</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Wykres 1"/>
+        <xdr:cNvPr id="6" name="Wykres 5"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1244,237 +1368,64 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C39"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="15.85546875" customWidth="1"/>
     <col min="2" max="2" width="10.42578125" customWidth="1"/>
+    <col min="4" max="4" width="20" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>7</v>
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>0.94</v>
+      </c>
+      <c r="C2">
+        <v>0.8</v>
+      </c>
+      <c r="D2">
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B2">
-        <v>0.92</v>
+      <c r="C3">
+        <v>0.63</v>
       </c>
-      <c r="C2">
-        <v>0.76068380000000002</v>
+      <c r="D3">
+        <v>0.48</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B3">
-        <v>0.86</v>
-      </c>
-      <c r="C3">
-        <v>0.76068380000000002</v>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C4">
-        <v>0.76068380000000002</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C5">
-        <v>0.76068380000000002</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C6">
-        <v>0.76068380000000002</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C7">
-        <v>0.76068380000000002</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8">
-        <v>0.76068380000000002</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C9">
-        <v>0.76068380000000002</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C10">
-        <v>0.76068380000000002</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C11">
-        <v>0.76068380000000002</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C12">
-        <v>0.76068380000000002</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C13">
-        <v>0.76068380000000002</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>2</v>
-      </c>
-      <c r="C14">
-        <v>0.76068380000000002</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C15">
-        <v>0.76068380000000002</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C16">
-        <v>0.76068380000000002</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C17">
-        <v>0.76068380000000002</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C18">
-        <v>0.76068380000000002</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C19">
-        <v>0.76068380000000002</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>3</v>
-      </c>
-      <c r="C20">
-        <v>0.76068380000000002</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C21">
-        <v>0.76068380000000002</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C22">
-        <v>0.76068380000000002</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C23">
-        <v>0.76068380000000002</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C24">
-        <v>0.76068380000000002</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C25">
-        <v>0.76068380000000002</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>5</v>
-      </c>
-      <c r="C26">
-        <v>0.76068380000000002</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C27">
-        <v>0.76068380000000002</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C28">
-        <v>0.76068380000000002</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C29">
-        <v>0.76068380000000002</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C30">
-        <v>0.76068380000000002</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C31">
-        <v>0.76068380000000002</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>6</v>
-      </c>
-      <c r="C32">
-        <v>0.76068380000000002</v>
-      </c>
-    </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C33">
-        <v>0.76068380000000002</v>
-      </c>
-    </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C34">
-        <v>0.76068380000000002</v>
-      </c>
-    </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C35">
-        <v>0.76068380000000002</v>
-      </c>
-    </row>
-    <row r="36" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C36">
-        <v>0.76068380000000002</v>
-      </c>
-    </row>
-    <row r="37" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C37">
-        <v>0.76068380000000002</v>
-      </c>
-    </row>
-    <row r="38" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C38">
-        <v>0.76068380000000002</v>
-      </c>
-    </row>
-    <row r="39" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C39">
-        <v>0.76068380000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>